<commit_message>
Adding linear regression analysis
</commit_message>
<xml_diff>
--- a/experiments/Linear Regression/butlerwithgasconsumption.xlsx
+++ b/experiments/Linear Regression/butlerwithgasconsumption.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcochran\Documents\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\anna\experiments\Linear Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA67D5F1-86C8-4A5A-AF60-B047E46D7D87}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7935"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="27660" windowHeight="18420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId1"/>
+    <sheet name="Data" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Assignment</t>
   </si>
@@ -37,15 +46,87 @@
   <si>
     <t>Gasoline Consumption</t>
   </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 99.0%</t>
+  </si>
+  <si>
+    <t>Upper 99.0%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +147,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -75,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,11 +172,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -100,6 +209,14 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +232,2694 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gasoline Consumption</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$301</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="300"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$C$2:$C$301</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="300"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>6.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6576-4EF3-8C62-00A9FEF28CE9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="798382552"/>
+        <c:axId val="798377632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="798382552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798377632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="798377632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="798382552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>17858</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>91678</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A86FB9B-8AFB-4AD2-8DF6-066C06F119B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -193,6 +2998,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -228,6 +3050,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,8 +3242,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E301"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F0EFE2-8A89-402C-A245-6FB2C7310330}">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.69406354037551321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.48172419807859163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.47823412533838017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.3980775451568617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="6">
+        <v>539.58081578526412</v>
+      </c>
+      <c r="D12" s="6">
+        <v>269.79040789263206</v>
+      </c>
+      <c r="E12" s="6">
+        <v>138.02697936014891</v>
+      </c>
+      <c r="F12" s="6">
+        <v>4.0954199786735653E-43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6">
+        <v>297</v>
+      </c>
+      <c r="C13" s="6">
+        <v>580.52238421473544</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.9546208222718364</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7">
+        <v>299</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1120.1031999999996</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>2.4930953851713231</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.33669895039196179</v>
+      </c>
+      <c r="D17" s="6">
+        <v>7.4045237808702185</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1.3670300677042532E-12</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1.8304773977884776</v>
+      </c>
+      <c r="G17" s="6">
+        <v>3.1557133725541684</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.620208757561763</v>
+      </c>
+      <c r="I17" s="6">
+        <v>3.3659820127808833</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6">
+        <v>7.470182516213747E-2</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1.4274551618188731E-2</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5.2332169275952527</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3.1544373002976172E-7</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4.6609742745409605E-2</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.10279390757886533</v>
+      </c>
+      <c r="H18" s="6">
+        <v>3.7695279082518872E-2</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.11170837124175606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7">
+        <v>-6.7506102482905533E-2</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.1527079277625433</v>
+      </c>
+      <c r="D19" s="7">
+        <v>-0.44206023532632632</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.65876733561584766</v>
+      </c>
+      <c r="F19" s="7">
+        <v>-0.3680327885139324</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0.23302058354812136</v>
+      </c>
+      <c r="H19" s="7">
+        <v>-0.46339895548620669</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.32838675052039568</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -419,7 +3513,7 @@
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -436,7 +3530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -452,8 +3546,12 @@
       <c r="E2" s="4">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>CORREL(B2:B301, C2:C301)</f>
+        <v>0.95714525563178965</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -469,8 +3567,12 @@
       <c r="E3" s="4">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>CORREL(B2:B301, D2:D301)</f>
+        <v>2.5797888536263185E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -487,7 +3589,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -504,7 +3606,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -521,7 +3623,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -538,7 +3640,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -555,7 +3657,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -572,7 +3674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -589,7 +3691,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -606,7 +3708,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f>A11+1</f>
         <v>11</v>
@@ -624,7 +3726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" ref="A13:A76" si="0">A12+1</f>
         <v>12</v>
@@ -642,7 +3744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -660,7 +3762,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -678,7 +3780,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5829,29 +8931,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>